<commit_message>
web update  2019-5-15 23:10:39
</commit_message>
<xml_diff>
--- a/doc/log/201708044226刘研.xlsx
+++ b/doc/log/201708044226刘研.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="146">
   <si>
     <t>周一</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -570,6 +570,38 @@
   </si>
   <si>
     <t>08:30--10:10 &amp; 16:00--17:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019年5月14日23:24:48</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019年5月15日22:39:24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周二</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周三</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>web的搭建</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22:00--01:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OSALS项目架构的搭建，web的完善，成功</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12:30--15:00 &amp; 17:00--21:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -896,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1430,6 +1462,34 @@
         <v>137</v>
       </c>
     </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>138</v>
+      </c>
+      <c r="B50" t="s">
+        <v>140</v>
+      </c>
+      <c r="C50" t="s">
+        <v>142</v>
+      </c>
+      <c r="D50" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>139</v>
+      </c>
+      <c r="B51" t="s">
+        <v>141</v>
+      </c>
+      <c r="C51" t="s">
+        <v>144</v>
+      </c>
+      <c r="D51" t="s">
+        <v>145</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cmt xpj lbw TEST  2019-5-16 21:10:14
</commit_message>
<xml_diff>
--- a/doc/log/201708044226刘研.xlsx
+++ b/doc/log/201708044226刘研.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="156">
   <si>
     <t>周一</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -618,6 +618,30 @@
   </si>
   <si>
     <t>23:00--01:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>崔梦婷Dao单表建立成功，TEST单表通过</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>19:30--19:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>邢朋举Service层通过，缺少TEST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20:00--20:20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20:30--21:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>李博文DaoTest AND ServiceTest均通过</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -944,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1520,6 +1544,30 @@
         <v>149</v>
       </c>
     </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C53" t="s">
+        <v>150</v>
+      </c>
+      <c r="D53" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
+        <v>152</v>
+      </c>
+      <c r="D54" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C55" t="s">
+        <v>155</v>
+      </c>
+      <c r="D55" t="s">
+        <v>154</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
lgb,hyh,cmt DaoTest AND ServiceTest均通过  2019-5-17 10:07:09
</commit_message>
<xml_diff>
--- a/doc/log/201708044226刘研.xlsx
+++ b/doc/log/201708044226刘研.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="162">
   <si>
     <t>周一</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -641,15 +641,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Service层ManagerTestCase的建立</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00:00--00:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019年5月17日10:04:46</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周五</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>李博文DaoTest AND ServiceTest均通过</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Service层ManagerTestCase的建立</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00:00--00:30</t>
+    <t>刘广部，胡颖慧，崔梦婷DaoTest AND ServiceTest均通过</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>09:00--10:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -693,9 +709,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -976,10 +993,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1570,7 +1587,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C55" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D55" t="s">
         <v>154</v>
@@ -1578,10 +1595,24 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C56" t="s">
+        <v>155</v>
+      </c>
+      <c r="D56" t="s">
         <v>156</v>
       </c>
-      <c r="D56" t="s">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>157</v>
+      </c>
+      <c r="B57" t="s">
+        <v>158</v>
+      </c>
+      <c r="C57" t="s">
+        <v>160</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
项目总查 通过 Update   2019-5-19 16:28:48
</commit_message>
<xml_diff>
--- a/doc/log/201708044226刘研.xlsx
+++ b/doc/log/201708044226刘研.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="176">
   <si>
     <t>周一</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -698,6 +698,30 @@
   </si>
   <si>
     <t>xxManagerTestCase总查通过</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019年5月19日16:23:43</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周日</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10:10--10:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>web层理解</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16:30--18:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目总查 通过</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1025,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1677,6 +1701,28 @@
         <v>168</v>
       </c>
     </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>170</v>
+      </c>
+      <c r="B61" t="s">
+        <v>171</v>
+      </c>
+      <c r="C61" t="s">
+        <v>175</v>
+      </c>
+      <c r="D61" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C62" t="s">
+        <v>173</v>
+      </c>
+      <c r="D62" t="s">
+        <v>174</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Push because of osals  2019-5-22 20:51:11
</commit_message>
<xml_diff>
--- a/doc/log/201708044226刘研.xlsx
+++ b/doc/log/201708044226刘研.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="190">
   <si>
     <t>周一</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -754,6 +754,30 @@
   </si>
   <si>
     <t>15:00--17:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019年5月22日20:42:42</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周三</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>浅入了解Ajax Json Restful</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目包名规范化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>08:30--10:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18:00--20:30</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1081,10 +1105,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1791,6 +1815,28 @@
         <v>183</v>
       </c>
     </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>184</v>
+      </c>
+      <c r="B66" t="s">
+        <v>185</v>
+      </c>
+      <c r="C66" t="s">
+        <v>186</v>
+      </c>
+      <c r="D66" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C67" t="s">
+        <v>187</v>
+      </c>
+      <c r="D67" t="s">
+        <v>189</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FoolNLTK 分词标注 2019-6-13 01:26:28
</commit_message>
<xml_diff>
--- a/doc/log/201708044226刘研.xlsx
+++ b/doc/log/201708044226刘研.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="293">
   <si>
     <t>周一</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1174,6 +1174,22 @@
   </si>
   <si>
     <t>编写《nlp项目-开发计划》</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FoolNLTK中文分词与词性标注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019年6月13日01:25:44</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周四</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00:50--01:20</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1501,10 +1517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2599,6 +2615,20 @@
         <v>287</v>
       </c>
     </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>290</v>
+      </c>
+      <c r="B101" t="s">
+        <v>291</v>
+      </c>
+      <c r="C101" t="s">
+        <v>289</v>
+      </c>
+      <c r="D101" t="s">
+        <v>292</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ansj POS tagging  2019-6-14 11:08:35
</commit_message>
<xml_diff>
--- a/doc/log/201708044226刘研.xlsx
+++ b/doc/log/201708044226刘研.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="301">
   <si>
     <t>周一</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1193,7 +1193,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2019年6月13日23:22:33</t>
+    <t>分词标注完善</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13:00--17:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019年6月14日11:07:17</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1201,11 +1209,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>分词标注完善</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>13:00--17:00</t>
+    <t>分词标注完善 Ansj POS tagging</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优化 实体 : Student</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>08:30--11:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>08:30--11:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1533,10 +1549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2646,17 +2662,33 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
+      <c r="C102" t="s">
         <v>293</v>
       </c>
-      <c r="B102" t="s">
+      <c r="D102" t="s">
         <v>294</v>
       </c>
-      <c r="C102" t="s">
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
         <v>295</v>
       </c>
-      <c r="D102" t="s">
+      <c r="B103" t="s">
         <v>296</v>
+      </c>
+      <c r="C103" t="s">
+        <v>297</v>
+      </c>
+      <c r="D103" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C104" t="s">
+        <v>298</v>
+      </c>
+      <c r="D104" t="s">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>